<commit_message>
update omits on re-ran samples
</commit_message>
<xml_diff>
--- a/June_Event/Porewaters/pw_raw_npoc_tn_data/20220629_Readme_NPOC_TN_COMPASS_TEMPEST_PW_MONTHLY_n69.xlsx
+++ b/June_Event/Porewaters/pw_raw_npoc_tn_data/20220629_Readme_NPOC_TN_COMPASS_TEMPEST_PW_MONTHLY_n69.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/opal_otenburg_pnnl_gov/Documents/Documents/GitHub/TEMPEST/June_Event/Porewaters/pw_raw_npoc_tn_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{BD6EF9B9-E56E-D748-A766-32E3577F6896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F30450E3-E745-4945-9199-DCD2CA2DEE64}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{BD6EF9B9-E56E-D748-A766-32E3577F6896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B356269-2AA1-E149-9E05-9B9EA4C4BDE6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{414E37C4-6C0F-AA42-8BD9-6BC73138264E}"/>
+    <workbookView xWindow="0" yWindow="3280" windowWidth="28800" windowHeight="16500" xr2:uid="{414E37C4-6C0F-AA42-8BD9-6BC73138264E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="121">
   <si>
     <t>Sample Name</t>
   </si>
@@ -146,9 +146,6 @@
     <t>TMP_FW_SOURCE_HR5_DOC</t>
   </si>
   <si>
-    <t>TMP_SW_SOURCE_HR6_DOC</t>
-  </si>
-  <si>
     <t>TMP_SW_SOURCE_HR5_DOC</t>
   </si>
   <si>
@@ -396,6 +393,12 @@
   </si>
   <si>
     <t>*two different glass thickness-&gt; explains differing vial wts</t>
+  </si>
+  <si>
+    <t>TMP_SW_SOURCE_HR7_DOC</t>
+  </si>
+  <si>
+    <t>only 1 peak- re-ran to get more peaks</t>
   </si>
 </sst>
 </file>
@@ -767,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19AEBD17-6CC0-ED44-B8EB-00F06462890B}">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1000,54 +1003,66 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>119</v>
       </c>
       <c r="B22">
         <v>30</v>
       </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>120</v>
+      </c>
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23">
         <v>31</v>
       </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>120</v>
+      </c>
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24">
         <v>32</v>
       </c>
       <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
         <v>39</v>
-      </c>
-      <c r="D24" t="s">
-        <v>40</v>
       </c>
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25">
         <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26">
         <v>34</v>
@@ -1058,7 +1073,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27">
         <v>35</v>
@@ -1066,7 +1081,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28">
         <v>36</v>
@@ -1074,7 +1089,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B29">
         <v>37</v>
@@ -1082,7 +1097,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30">
         <v>38</v>
@@ -1090,850 +1105,850 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B32">
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B33">
         <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34">
         <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B35">
         <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B36">
         <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B37">
         <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B38">
         <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B39">
         <v>46</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40">
         <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41">
         <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42">
         <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B44">
         <v>50</v>
       </c>
       <c r="C44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B45">
         <v>51</v>
       </c>
       <c r="C45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B46">
         <v>52</v>
       </c>
       <c r="C46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B47">
         <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48">
         <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B49">
         <v>55</v>
       </c>
       <c r="C49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B50">
         <v>56</v>
       </c>
       <c r="C50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B51">
         <v>57</v>
       </c>
       <c r="C51" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B52">
         <v>58</v>
       </c>
       <c r="C52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B53">
         <v>59</v>
       </c>
       <c r="C53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B54">
         <v>60</v>
       </c>
       <c r="C54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B56">
         <v>61</v>
       </c>
       <c r="C56" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B57">
         <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B58">
         <v>63</v>
       </c>
       <c r="C58" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B59">
         <v>64</v>
       </c>
       <c r="C59" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B60">
         <v>65</v>
       </c>
       <c r="C60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D60" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B61">
         <v>66</v>
       </c>
       <c r="C61" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D61" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B62">
         <v>67</v>
       </c>
       <c r="C62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D62" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B63">
         <v>68</v>
       </c>
       <c r="C63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B64">
         <v>69</v>
       </c>
       <c r="C64" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D64" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B65">
         <v>70</v>
       </c>
       <c r="C65" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D65" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B66">
         <v>71</v>
       </c>
       <c r="C66" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D66" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="C67" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B68">
         <v>72</v>
       </c>
       <c r="C68" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B69">
         <v>73</v>
       </c>
       <c r="C69" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D69" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B70">
         <v>74</v>
       </c>
       <c r="C70" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D70" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B71">
         <v>75</v>
       </c>
       <c r="C71" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D71" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B72">
         <v>76</v>
       </c>
       <c r="C72" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D72" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B73">
         <v>77</v>
       </c>
       <c r="C73" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D73" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B74">
         <v>78</v>
       </c>
       <c r="C74" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D74" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B75">
         <v>79</v>
       </c>
       <c r="C75" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D75" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B76">
         <v>80</v>
       </c>
       <c r="C76" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D76" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B77">
         <v>81</v>
       </c>
       <c r="C77" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B78">
         <v>82</v>
       </c>
       <c r="C78" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D78" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B79">
         <v>0</v>
       </c>
       <c r="C79" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D79" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B80">
         <v>83</v>
       </c>
       <c r="C80" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D80" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B81">
         <v>84</v>
       </c>
       <c r="C81" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D81" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B82">
         <v>85</v>
       </c>
       <c r="C82" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B83">
         <v>86</v>
       </c>
       <c r="C83" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D83" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B84">
         <v>87</v>
       </c>
       <c r="C84" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D84" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B85">
         <v>88</v>
       </c>
       <c r="C85" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D85" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B86">
         <v>89</v>
       </c>
       <c r="C86" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D86" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B87">
         <v>90</v>
       </c>
       <c r="C87" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D87" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B88">
         <v>91</v>
       </c>
       <c r="C88" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D88" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B89">
         <v>92</v>
       </c>
       <c r="C89" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D89" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B90">
         <v>0</v>
       </c>
       <c r="C90" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D90" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B91">
         <v>93</v>
       </c>
       <c r="C91" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D91" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1960,28 +1975,28 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" t="s">
         <v>118</v>
-      </c>
-      <c r="J1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2055,6 +2070,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007324DF9BA5F6B948938C142504C8F34F" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c4aadcd1f2a12dc9b07f6546b5e76248">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="da8c28ad-5ac5-4047-b08a-f75bc24d91a9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6457694f174ba676422feeebbff24cf4" ns2:_="">
     <xsd:import namespace="da8c28ad-5ac5-4047-b08a-f75bc24d91a9"/>
@@ -2224,16 +2248,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D4F60B5-3874-4179-8D73-4352AEBE626B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A701949D-1257-47EA-88EF-D14148793769}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2249,12 +2272,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D4F60B5-3874-4179-8D73-4352AEBE626B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>